<commit_message>
ajout de 2 fonctions
fonction qui corrige les fautes d'orthographe en francais et une autre fonction qui traduit puis corrige
</commit_message>
<xml_diff>
--- a/cv.xlsx
+++ b/cv.xlsx
@@ -16,130 +16,130 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
-    <t>Nicolas Buissart</t>
-  </si>
-  <si>
-    <t>Beauchamp (95) - Email me on Indeed: indeed.com/r/Nicolas-Buissart/abab6e2e9d3337e8</t>
-  </si>
-  <si>
-    <t>EXPÉRIENCE</t>
-  </si>
-  <si>
-    <t>Data Scientist ( Stage )</t>
-  </si>
-  <si>
-    <t>Société Générale  -  Hauts-de-Seine -</t>
+    <t>nicolas buissart</t>
+  </si>
+  <si>
+    <t>beauchamp (95) - email me on indeed: indeed.com/r/nicolas-buissart/abab6e2e9d3337e8</t>
+  </si>
+  <si>
+    <t>expÉrience</t>
+  </si>
+  <si>
+    <t>data scientist ( stage )</t>
+  </si>
+  <si>
+    <t>société générale  -  hauts-de-seine -</t>
   </si>
   <si>
     <t>juin 2017 - novembre 2017</t>
   </si>
   <si>
-    <t>Au cours de ce stage j’ai travaillé sur la réconciliation automatique de la comptabilité économique et de gestion.</t>
-  </si>
-  <si>
-    <t>Mise en place de deux modèles de détection d’écart,un basé sur un système de scoring de la rareté des</t>
-  </si>
-  <si>
-    <t>écarts, le deuxième détecte les écarts récurrents. J’ai pu travailler sur des modèles tel que: RandomForest,</t>
-  </si>
-  <si>
-    <t>GradientBoost  Regression  et  Logistic  Regression.  Langages  utilisés:  Python(les  modules  Scikit-Learn  et</t>
-  </si>
-  <si>
-    <t>Pandas) Logiciel: Tableau pour valider les modèles et mise en place de KPI</t>
-  </si>
-  <si>
-    <t>Stagiaire</t>
-  </si>
-  <si>
-    <t>Humbrain  -  Paris (75) -</t>
+    <t>au cours de ce stage j’ai travaillé sur la réconciliation automatique de la comptabilité économique et de gestion.</t>
+  </si>
+  <si>
+    <t>mise en place de deux modèles de détection d’écart,un basé sur un système de scoring de la rareté des</t>
+  </si>
+  <si>
+    <t>écarts, le deuxième détecte les écarts récurrents. j’ai pu travailler sur des modèles tel que: randomforest,</t>
+  </si>
+  <si>
+    <t>gradientboost  regression  et  logistic  regression.  langages  utilisés:  python(les  modules  scikit-learn  et</t>
+  </si>
+  <si>
+    <t>pandas) logiciel: tableau pour valider les modèles et mise en place de kpi</t>
+  </si>
+  <si>
+    <t>stagiaire</t>
+  </si>
+  <si>
+    <t>humbrain  -  paris (75) -</t>
   </si>
   <si>
     <t>mai 2016 - septembre 2016</t>
   </si>
   <si>
-    <t>Stagiaire Humbrain</t>
-  </si>
-  <si>
-    <t>Humbrain est une entreprise réalisant des prestations comme la mise en place de services au sein d'entreprise</t>
-  </si>
-  <si>
-    <t>J'ai réalise les missions suivantes</t>
-  </si>
-  <si>
-    <t>Mail auprès de l'entreprise Humbrain:</t>
-  </si>
-  <si>
-    <t>buissartni@ • Création et Mise à jour du site Web de la société.</t>
-  </si>
-  <si>
-    <t>eisti.eu • Mise en place de trois indicateurs sur les différents services fourni par l'entreprise afin de savoir l'état</t>
+    <t>stagiaire humbrain</t>
+  </si>
+  <si>
+    <t>humbrain est une entreprise réalisant des prestations comme la mise en place de services au sein d'entreprise</t>
+  </si>
+  <si>
+    <t>j'ai réalise les missions suivantes</t>
+  </si>
+  <si>
+    <t>mail auprès de l'entreprise humbrain:</t>
+  </si>
+  <si>
+    <t>buissartni@ • création et mise à jour du site web de la société.</t>
+  </si>
+  <si>
+    <t>eisti.eu • mise en place de trois indicateurs sur les différents services fourni par l'entreprise afin de savoir l'état</t>
   </si>
   <si>
     <t>de ces-derniers.</t>
   </si>
   <si>
-    <t>• Mise en place d'un tableau de bord.</t>
-  </si>
-  <si>
-    <t>Programmation • Participation aux réunions avec les clients.</t>
-  </si>
-  <si>
-    <t>• Réflexion autour de l'amélioration de certains algorithmes.</t>
-  </si>
-  <si>
-    <t>Gérant</t>
-  </si>
-  <si>
-    <t>Youtube -</t>
+    <t>• mise en place d'un tableau de bord.</t>
+  </si>
+  <si>
+    <t>programmation • participation aux réunions avec les clients.</t>
+  </si>
+  <si>
+    <t>• réflexion autour de l'amélioration de certains algorithmes.</t>
+  </si>
+  <si>
+    <t>gérant</t>
+  </si>
+  <si>
+    <t>youtube -</t>
   </si>
   <si>
     <t>mai 2011 - septembre 2013</t>
   </si>
   <si>
-    <t>J'ai été gérant d'une chaine YouTube pendant deux ans j'ai totalisé plus de deux millions de vues pendant</t>
-  </si>
-  <si>
-    <t>cette période. Cela m'a appris à être sérieux et ordonné dans mon travail.</t>
-  </si>
-  <si>
-    <t>FORMATION</t>
-  </si>
-  <si>
-    <t>Diplôme d'ingénieur en voix</t>
-  </si>
-  <si>
-    <t>Ecole internationale des Sciences du Traitement de l'Information  -  Cergy (95)</t>
+    <t>j'ai été gérant d'une chaine youtube pendant deux ans j'ai totalisé plus de deux millions de vues pendant</t>
+  </si>
+  <si>
+    <t>cette période. cela m'a appris à être sérieux et ordonné dans mon travail.</t>
+  </si>
+  <si>
+    <t>formation</t>
+  </si>
+  <si>
+    <t>diplôme d'ingénieur en voix</t>
+  </si>
+  <si>
+    <t>ecole internationale des sciences du traitement de l'information  -  cergy (95)</t>
   </si>
   <si>
     <t>2012 - 2017</t>
   </si>
   <si>
-    <t>_x000C_COMPÉTENCE</t>
-  </si>
-  <si>
-    <t>Scala, Python, R, SQL, Spark, Anglais TOEIC 870</t>
-  </si>
-  <si>
-    <t>INFORMATIONS COMPLÉMENTAIRES</t>
-  </si>
-  <si>
-    <t>Compétences l'aide d'un Random Forest.</t>
-  </si>
-  <si>
-    <t>• Analyse des Tweets avec Tweepy - python: Similarité entre les</t>
-  </si>
-  <si>
-    <t>retweets en rapport avec Obama et Trump ( utilisation de la libraire pan-</t>
+    <t>_x000C_compÉtence</t>
+  </si>
+  <si>
+    <t>scala, python, r, sql, spark, anglais toeic 870</t>
+  </si>
+  <si>
+    <t>informations complÉmentaires</t>
+  </si>
+  <si>
+    <t>compétences l'aide d'un random forest.</t>
+  </si>
+  <si>
+    <t>• analyse des tweets avec tweepy - python: similarité entre les</t>
+  </si>
+  <si>
+    <t>retweets en rapport avec obama et trump ( utilisation de la libraire pan-</t>
   </si>
   <si>
     <t>das).</t>
   </si>
   <si>
-    <t>• Projet de Text-Mining sur les différents programmes présidentiels de</t>
-  </si>
-  <si>
-    <t>2017: Machine learning sur les programmes présidentiels, apprentis-</t>
+    <t>• projet de text-mining sur les différents programmes présidentiels de</t>
+  </si>
+  <si>
+    <t>2017: machine learning sur les programmes présidentiels, apprentis-</t>
   </si>
   <si>
     <t>sage sur les programmes de 2012 afin de prédire le bord politique d'un</t>
@@ -148,25 +148,25 @@
     <t>programme quelconque de 2017.</t>
   </si>
   <si>
-    <t>• Analyse de série temporelle.</t>
-  </si>
-  <si>
-    <t>• Projet Spark sur un système de recommendation.</t>
-  </si>
-  <si>
-    <t>En plus de ma formation je suis des cours sur Data Camp:</t>
-  </si>
-  <si>
-    <t>• Text Mining: Bag of Words</t>
-  </si>
-  <si>
-    <t>• Manipulating DataFrames with pandas</t>
-  </si>
-  <si>
-    <t>• Python Data Science Toolbox</t>
-  </si>
-  <si>
-    <t>• Financial Trading in R.</t>
+    <t>• analyse de série temporelle.</t>
+  </si>
+  <si>
+    <t>• projet spark sur un système de recommendation.</t>
+  </si>
+  <si>
+    <t>en plus de ma formation je suis des cours sur data camp:</t>
+  </si>
+  <si>
+    <t>• text mining: bag of words</t>
+  </si>
+  <si>
+    <t>• manipulating dataframes with pandas</t>
+  </si>
+  <si>
+    <t>• python data science toolbox</t>
+  </si>
+  <si>
+    <t>• financial trading in r.</t>
   </si>
   <si>
     <t>_x000C_</t>

</xml_diff>

<commit_message>
update gitignore for results cv.txt & cv.xlsx
</commit_message>
<xml_diff>
--- a/cv.xlsx
+++ b/cv.xlsx
@@ -16,130 +16,130 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
-    <t>Nicolas Buissart</t>
-  </si>
-  <si>
-    <t>Beauchamp (95) - Email me on Indeed: indeed.com/r/Nicolas-Buissart/abab6e2e9d3337e8</t>
-  </si>
-  <si>
-    <t>EXPÉRIENCE</t>
-  </si>
-  <si>
-    <t>Data Scientist ( Stage )</t>
-  </si>
-  <si>
-    <t>Société Générale  -  Hauts-de-Seine -</t>
+    <t>nicolas buissart</t>
+  </si>
+  <si>
+    <t>beauchamp (95) - email me on indeed: indeed.com/r/nicolas-buissart/abab6e2e9d3337e8</t>
+  </si>
+  <si>
+    <t>expÉrience</t>
+  </si>
+  <si>
+    <t>data scientist ( stage )</t>
+  </si>
+  <si>
+    <t>société générale  -  hauts-de-seine -</t>
   </si>
   <si>
     <t>juin 2017 - novembre 2017</t>
   </si>
   <si>
-    <t>Au cours de ce stage j’ai travaillé sur la réconciliation automatique de la comptabilité économique et de gestion.</t>
-  </si>
-  <si>
-    <t>Mise en place de deux modèles de détection d’écart,un basé sur un système de scoring de la rareté des</t>
-  </si>
-  <si>
-    <t>écarts, le deuxième détecte les écarts récurrents. J’ai pu travailler sur des modèles tel que: RandomForest,</t>
-  </si>
-  <si>
-    <t>GradientBoost  Regression  et  Logistic  Regression.  Langages  utilisés:  Python(les  modules  Scikit-Learn  et</t>
-  </si>
-  <si>
-    <t>Pandas) Logiciel: Tableau pour valider les modèles et mise en place de KPI</t>
-  </si>
-  <si>
-    <t>Stagiaire</t>
-  </si>
-  <si>
-    <t>Humbrain  -  Paris (75) -</t>
+    <t>au cours de ce stage j’ai travaillé sur la réconciliation automatique de la comptabilité économique et de gestion.</t>
+  </si>
+  <si>
+    <t>mise en place de deux modèles de détection d’écart,un basé sur un système de scoring de la rareté des</t>
+  </si>
+  <si>
+    <t>écarts, le deuxième détecte les écarts récurrents. j’ai pu travailler sur des modèles tel que: randomforest,</t>
+  </si>
+  <si>
+    <t>gradientboost  regression  et  logistic  regression.  langages  utilisés:  python(les  modules  scikit-learn  et</t>
+  </si>
+  <si>
+    <t>pandas) logiciel: tableau pour valider les modèles et mise en place de kpi</t>
+  </si>
+  <si>
+    <t>stagiaire</t>
+  </si>
+  <si>
+    <t>humbrain  -  paris (75) -</t>
   </si>
   <si>
     <t>mai 2016 - septembre 2016</t>
   </si>
   <si>
-    <t>Stagiaire Humbrain</t>
-  </si>
-  <si>
-    <t>Humbrain est une entreprise réalisant des prestations comme la mise en place de services au sein d'entreprise</t>
-  </si>
-  <si>
-    <t>J'ai réalise les missions suivantes</t>
-  </si>
-  <si>
-    <t>Mail auprès de l'entreprise Humbrain:</t>
-  </si>
-  <si>
-    <t>buissartni@ • Création et Mise à jour du site Web de la société.</t>
-  </si>
-  <si>
-    <t>eisti.eu • Mise en place de trois indicateurs sur les différents services fourni par l'entreprise afin de savoir l'état</t>
+    <t>stagiaire humbrain</t>
+  </si>
+  <si>
+    <t>humbrain est une entreprise réalisant des prestations comme la mise en place de services au sein d'entreprise</t>
+  </si>
+  <si>
+    <t>j'ai réalise les missions suivantes</t>
+  </si>
+  <si>
+    <t>mail auprès de l'entreprise humbrain:</t>
+  </si>
+  <si>
+    <t>buissartni@ • création et mise à jour du site web de la société.</t>
+  </si>
+  <si>
+    <t>eisti.eu • mise en place de trois indicateurs sur les différents services fourni par l'entreprise afin de savoir l'état</t>
   </si>
   <si>
     <t>de ces-derniers.</t>
   </si>
   <si>
-    <t>• Mise en place d'un tableau de bord.</t>
-  </si>
-  <si>
-    <t>Programmation • Participation aux réunions avec les clients.</t>
-  </si>
-  <si>
-    <t>• Réflexion autour de l'amélioration de certains algorithmes.</t>
-  </si>
-  <si>
-    <t>Gérant</t>
-  </si>
-  <si>
-    <t>Youtube -</t>
+    <t>• mise en place d'un tableau de bord.</t>
+  </si>
+  <si>
+    <t>programmation • participation aux réunions avec les clients.</t>
+  </si>
+  <si>
+    <t>• réflexion autour de l'amélioration de certains algorithmes.</t>
+  </si>
+  <si>
+    <t>gérant</t>
+  </si>
+  <si>
+    <t>youtube -</t>
   </si>
   <si>
     <t>mai 2011 - septembre 2013</t>
   </si>
   <si>
-    <t>J'ai été gérant d'une chaine YouTube pendant deux ans j'ai totalisé plus de deux millions de vues pendant</t>
-  </si>
-  <si>
-    <t>cette période. Cela m'a appris à être sérieux et ordonné dans mon travail.</t>
-  </si>
-  <si>
-    <t>FORMATION</t>
-  </si>
-  <si>
-    <t>Diplôme d'ingénieur en voix</t>
-  </si>
-  <si>
-    <t>Ecole internationale des Sciences du Traitement de l'Information  -  Cergy (95)</t>
+    <t>j'ai été gérant d'une chaine youtube pendant deux ans j'ai totalisé plus de deux millions de vues pendant</t>
+  </si>
+  <si>
+    <t>cette période. cela m'a appris à être sérieux et ordonné dans mon travail.</t>
+  </si>
+  <si>
+    <t>formation</t>
+  </si>
+  <si>
+    <t>diplôme d'ingénieur en voix</t>
+  </si>
+  <si>
+    <t>ecole internationale des sciences du traitement de l'information  -  cergy (95)</t>
   </si>
   <si>
     <t>2012 - 2017</t>
   </si>
   <si>
-    <t>_x000C_COMPÉTENCE</t>
-  </si>
-  <si>
-    <t>Scala, Python, R, SQL, Spark, Anglais TOEIC 870</t>
-  </si>
-  <si>
-    <t>INFORMATIONS COMPLÉMENTAIRES</t>
-  </si>
-  <si>
-    <t>Compétences l'aide d'un Random Forest.</t>
-  </si>
-  <si>
-    <t>• Analyse des Tweets avec Tweepy - python: Similarité entre les</t>
-  </si>
-  <si>
-    <t>retweets en rapport avec Obama et Trump ( utilisation de la libraire pan-</t>
+    <t>_x000C_compÉtence</t>
+  </si>
+  <si>
+    <t>scala, python, r, sql, spark, anglais toeic 870</t>
+  </si>
+  <si>
+    <t>informations complÉmentaires</t>
+  </si>
+  <si>
+    <t>compétences l'aide d'un random forest.</t>
+  </si>
+  <si>
+    <t>• analyse des tweets avec tweepy - python: similarité entre les</t>
+  </si>
+  <si>
+    <t>retweets en rapport avec obama et trump ( utilisation de la libraire pan-</t>
   </si>
   <si>
     <t>das).</t>
   </si>
   <si>
-    <t>• Projet de Text-Mining sur les différents programmes présidentiels de</t>
-  </si>
-  <si>
-    <t>2017: Machine learning sur les programmes présidentiels, apprentis-</t>
+    <t>• projet de text-mining sur les différents programmes présidentiels de</t>
+  </si>
+  <si>
+    <t>2017: machine learning sur les programmes présidentiels, apprentis-</t>
   </si>
   <si>
     <t>sage sur les programmes de 2012 afin de prédire le bord politique d'un</t>
@@ -148,25 +148,25 @@
     <t>programme quelconque de 2017.</t>
   </si>
   <si>
-    <t>• Analyse de série temporelle.</t>
-  </si>
-  <si>
-    <t>• Projet Spark sur un système de recommendation.</t>
-  </si>
-  <si>
-    <t>En plus de ma formation je suis des cours sur Data Camp:</t>
-  </si>
-  <si>
-    <t>• Text Mining: Bag of Words</t>
-  </si>
-  <si>
-    <t>• Manipulating DataFrames with pandas</t>
-  </si>
-  <si>
-    <t>• Python Data Science Toolbox</t>
-  </si>
-  <si>
-    <t>• Financial Trading in R.</t>
+    <t>• analyse de série temporelle.</t>
+  </si>
+  <si>
+    <t>• projet spark sur un système de recommendation.</t>
+  </si>
+  <si>
+    <t>en plus de ma formation je suis des cours sur data camp:</t>
+  </si>
+  <si>
+    <t>• text mining: bag of words</t>
+  </si>
+  <si>
+    <t>• manipulating dataframes with pandas</t>
+  </si>
+  <si>
+    <t>• python data science toolbox</t>
+  </si>
+  <si>
+    <t>• financial trading in r.</t>
   </si>
   <si>
     <t>_x000C_</t>

</xml_diff>